<commit_message>
Add local authority HQ postcode
</commit_message>
<xml_diff>
--- a/lookups/la_websites.xlsx
+++ b/lookups/la_websites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Sharing folder\School_dashboard_code (alice)\data\la_websites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Sharing folder\Alice\lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Aberdeen City</t>
   </si>
@@ -234,6 +234,99 @@
   </si>
   <si>
     <t>Grant aided</t>
+  </si>
+  <si>
+    <t>EH1</t>
+  </si>
+  <si>
+    <t>AB10</t>
+  </si>
+  <si>
+    <t>DD8</t>
+  </si>
+  <si>
+    <t>PA20</t>
+  </si>
+  <si>
+    <t>FK10</t>
+  </si>
+  <si>
+    <t>DG1</t>
+  </si>
+  <si>
+    <t>DD1</t>
+  </si>
+  <si>
+    <t>KA3</t>
+  </si>
+  <si>
+    <t>G66</t>
+  </si>
+  <si>
+    <t>EH41</t>
+  </si>
+  <si>
+    <t>G46</t>
+  </si>
+  <si>
+    <t>HS1</t>
+  </si>
+  <si>
+    <t>FK1</t>
+  </si>
+  <si>
+    <t>KY11</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>AB3</t>
+  </si>
+  <si>
+    <t>PA15</t>
+  </si>
+  <si>
+    <t>EH22</t>
+  </si>
+  <si>
+    <t>KA12</t>
+  </si>
+  <si>
+    <t>ML1</t>
+  </si>
+  <si>
+    <t>KW15</t>
+  </si>
+  <si>
+    <t>KY13</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>EH26</t>
+  </si>
+  <si>
+    <t>ZE1</t>
+  </si>
+  <si>
+    <t>KA7</t>
+  </si>
+  <si>
+    <t>ML3</t>
+  </si>
+  <si>
+    <t>G63</t>
+  </si>
+  <si>
+    <t>G82</t>
+  </si>
+  <si>
+    <t>EH54</t>
+  </si>
+  <si>
+    <t>postcode</t>
   </si>
 </sst>
 </file>
@@ -551,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,7 +654,7 @@
     <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -571,8 +664,11 @@
       <c r="C1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -582,8 +678,11 @@
       <c r="C2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -591,7 +690,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -601,8 +700,11 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -612,8 +714,11 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -623,8 +728,11 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -634,8 +742,11 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -645,8 +756,11 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -656,8 +770,11 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -667,8 +784,11 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -678,8 +798,11 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -689,8 +812,11 @@
       <c r="C12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -700,8 +826,11 @@
       <c r="C13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -711,8 +840,11 @@
       <c r="C14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -722,8 +854,11 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -733,8 +868,11 @@
       <c r="C16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -744,8 +882,11 @@
       <c r="C17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -755,8 +896,11 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -766,8 +910,11 @@
       <c r="C19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -777,8 +924,11 @@
       <c r="C20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -788,8 +938,11 @@
       <c r="C21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -799,8 +952,11 @@
       <c r="C22" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -810,8 +966,11 @@
       <c r="C23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -821,8 +980,11 @@
       <c r="C24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -832,8 +994,11 @@
       <c r="C25" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -843,8 +1008,11 @@
       <c r="C26" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -854,8 +1022,11 @@
       <c r="C27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -865,8 +1036,11 @@
       <c r="C28" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -876,8 +1050,11 @@
       <c r="C29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -887,8 +1064,11 @@
       <c r="C30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -898,8 +1078,11 @@
       <c r="C31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -909,8 +1092,11 @@
       <c r="C32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -920,8 +1106,11 @@
       <c r="C33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -931,8 +1120,11 @@
       <c r="C34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -941,6 +1133,9 @@
       </c>
       <c r="C35" t="s">
         <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>